<commit_message>
Update DEG Number of Identified Genes.xlsx
</commit_message>
<xml_diff>
--- a/DEG_data/DEG Number of Identified Genes.xlsx
+++ b/DEG_data/DEG Number of Identified Genes.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vicky\Documents\GitHub\snRNA-seq-pipeline\DEG_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2D5B1C-C9D6-4F45-A7F0-F161C89AA8D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22676E7A-98C6-498E-8A6C-3C7ACE5579B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{069C3F11-75A4-4FB6-B215-0854D8E6AA19}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{069C3F11-75A4-4FB6-B215-0854D8E6AA19}"/>
   </bookViews>
   <sheets>
-    <sheet name="Num Stat Sig Genes Identified" sheetId="1" r:id="rId1"/>
+    <sheet name="M_MUT_and_WT_M_P30_CORT" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -490,7 +490,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A11" sqref="A11:K12"/>
+      <selection pane="topRight" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
update DEGs identified for E18
</commit_message>
<xml_diff>
--- a/DEG_data/DEG Number of Identified Genes.xlsx
+++ b/DEG_data/DEG Number of Identified Genes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vicky\Documents\GitHub\snRNA-seq-pipeline\DEG_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B096297-2983-4F3F-8534-402E99A74801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1506E523-AFAD-4A58-9E8C-7ED4B15A1BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{069C3F11-75A4-4FB6-B215-0854D8E6AA19}"/>
   </bookViews>
@@ -161,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -176,9 +176,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -502,12 +499,13 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
@@ -523,7 +521,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -558,373 +556,566 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="6">
         <f>E2+H2+I2+K2</f>
-        <v>0</v>
-      </c>
-      <c r="C2" s="7">
+        <v>4</v>
+      </c>
+      <c r="C2" s="6">
         <f>F2+H2+J2+K2</f>
-        <v>0</v>
-      </c>
-      <c r="D2" s="7">
+        <v>593</v>
+      </c>
+      <c r="D2" s="6">
         <f>G2+J2+I2+K2</f>
-        <v>0</v>
-      </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="6"/>
+        <v>562</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0</v>
+      </c>
+      <c r="F2" s="6">
+        <v>193</v>
+      </c>
+      <c r="G2" s="6">
+        <v>162</v>
+      </c>
+      <c r="H2" s="6">
+        <v>0</v>
+      </c>
+      <c r="I2" s="6">
+        <v>0</v>
+      </c>
+      <c r="J2" s="6">
+        <v>396</v>
+      </c>
+      <c r="K2" s="3">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="6">
         <f t="shared" ref="B3:B15" si="0">E3+H3+I3+K3</f>
-        <v>0</v>
-      </c>
-      <c r="C3" s="7">
+        <v>4</v>
+      </c>
+      <c r="C3" s="6">
         <f t="shared" ref="C3:C15" si="1">F3+H3+J3+K3</f>
-        <v>0</v>
-      </c>
-      <c r="D3" s="7">
+        <v>291</v>
+      </c>
+      <c r="D3" s="6">
         <f t="shared" ref="D3:D15" si="2">G3+J3+I3+K3</f>
-        <v>0</v>
-      </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="6"/>
+        <v>280</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0</v>
+      </c>
+      <c r="F3" s="6">
+        <v>128</v>
+      </c>
+      <c r="G3" s="6">
+        <v>116</v>
+      </c>
+      <c r="H3" s="6">
+        <v>0</v>
+      </c>
+      <c r="I3" s="6">
+        <v>1</v>
+      </c>
+      <c r="J3" s="6">
+        <v>160</v>
+      </c>
+      <c r="K3" s="3">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C4" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D4" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="6"/>
+      <c r="B4" s="6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C4" s="6">
+        <f t="shared" si="1"/>
+        <v>163</v>
+      </c>
+      <c r="D4" s="6">
+        <f t="shared" si="2"/>
+        <v>191</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0</v>
+      </c>
+      <c r="F4" s="6">
+        <v>68</v>
+      </c>
+      <c r="G4" s="6">
+        <v>96</v>
+      </c>
+      <c r="H4" s="6">
+        <v>0</v>
+      </c>
+      <c r="I4" s="6">
+        <v>0</v>
+      </c>
+      <c r="J4" s="6">
+        <v>92</v>
+      </c>
+      <c r="K4" s="3">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C5" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D5" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="6"/>
+      <c r="B5" s="6">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="C5" s="6">
+        <f t="shared" si="1"/>
+        <v>642</v>
+      </c>
+      <c r="D5" s="6">
+        <f t="shared" si="2"/>
+        <v>705</v>
+      </c>
+      <c r="E5" s="6">
+        <v>1</v>
+      </c>
+      <c r="F5" s="6">
+        <v>133</v>
+      </c>
+      <c r="G5" s="6">
+        <v>195</v>
+      </c>
+      <c r="H5" s="6">
+        <v>0</v>
+      </c>
+      <c r="I5" s="6">
+        <v>1</v>
+      </c>
+      <c r="J5" s="6">
+        <v>492</v>
+      </c>
+      <c r="K5" s="3">
+        <v>17</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C6" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D6" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="6"/>
+      <c r="B6" s="6">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C6" s="6">
+        <f t="shared" si="1"/>
+        <v>406</v>
+      </c>
+      <c r="D6" s="6">
+        <f t="shared" si="2"/>
+        <v>704</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0</v>
+      </c>
+      <c r="F6" s="6">
+        <v>72</v>
+      </c>
+      <c r="G6" s="6">
+        <v>367</v>
+      </c>
+      <c r="H6" s="6">
+        <v>0</v>
+      </c>
+      <c r="I6" s="6">
+        <v>3</v>
+      </c>
+      <c r="J6" s="6">
+        <v>321</v>
+      </c>
+      <c r="K6" s="3">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C7" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D7" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="6"/>
+      <c r="B7" s="6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C7" s="6">
+        <f t="shared" si="1"/>
+        <v>66</v>
+      </c>
+      <c r="D7" s="6">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="E7" s="6">
+        <v>0</v>
+      </c>
+      <c r="F7" s="6">
+        <v>28</v>
+      </c>
+      <c r="G7" s="6">
+        <v>61</v>
+      </c>
+      <c r="H7" s="6">
+        <v>0</v>
+      </c>
+      <c r="I7" s="6">
+        <v>1</v>
+      </c>
+      <c r="J7" s="6">
+        <v>36</v>
+      </c>
+      <c r="K7" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C8" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D8" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
+      <c r="B8" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C8" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D8" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0</v>
+      </c>
+      <c r="F8" s="6">
+        <v>0</v>
+      </c>
+      <c r="G8" s="6">
+        <v>0</v>
+      </c>
+      <c r="H8" s="6">
+        <v>0</v>
+      </c>
+      <c r="I8" s="6">
+        <v>0</v>
+      </c>
+      <c r="J8" s="6">
+        <v>0</v>
+      </c>
+      <c r="K8" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C9" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D9" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
+      <c r="B9" s="6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C9" s="6">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="D9" s="6">
+        <f t="shared" si="2"/>
+        <v>114</v>
+      </c>
+      <c r="E9" s="6">
+        <v>0</v>
+      </c>
+      <c r="F9" s="6">
+        <v>3</v>
+      </c>
+      <c r="G9" s="6">
+        <v>101</v>
+      </c>
+      <c r="H9" s="6">
+        <v>0</v>
+      </c>
+      <c r="I9" s="6">
+        <v>2</v>
+      </c>
+      <c r="J9" s="6">
+        <v>9</v>
+      </c>
+      <c r="K9" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C10" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D10" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
+      <c r="B10" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C10" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D10" s="6">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="E10" s="6">
+        <v>0</v>
+      </c>
+      <c r="F10" s="6">
+        <v>0</v>
+      </c>
+      <c r="G10" s="6">
+        <v>5</v>
+      </c>
+      <c r="H10" s="6">
+        <v>0</v>
+      </c>
+      <c r="I10" s="6">
+        <v>0</v>
+      </c>
+      <c r="J10" s="6">
+        <v>1</v>
+      </c>
+      <c r="K10" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C11" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D11" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
+      <c r="B11" s="6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C11" s="6">
+        <f t="shared" si="1"/>
+        <v>222</v>
+      </c>
+      <c r="D11" s="6">
+        <f t="shared" si="2"/>
+        <v>658</v>
+      </c>
+      <c r="E11" s="6">
+        <v>0</v>
+      </c>
+      <c r="F11" s="6">
+        <v>29</v>
+      </c>
+      <c r="G11" s="6">
+        <v>465</v>
+      </c>
+      <c r="H11" s="6">
+        <v>0</v>
+      </c>
+      <c r="I11" s="6">
+        <v>0</v>
+      </c>
+      <c r="J11" s="6">
+        <v>189</v>
+      </c>
+      <c r="K11" s="4">
+        <v>4</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C12" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D12" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
+      <c r="B12" s="6">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="C12" s="6">
+        <f t="shared" si="1"/>
+        <v>516</v>
+      </c>
+      <c r="D12" s="6">
+        <f t="shared" si="2"/>
+        <v>824</v>
+      </c>
+      <c r="E12" s="6">
+        <v>0</v>
+      </c>
+      <c r="F12" s="6">
+        <v>101</v>
+      </c>
+      <c r="G12" s="6">
+        <v>405</v>
+      </c>
+      <c r="H12" s="6">
+        <v>0</v>
+      </c>
+      <c r="I12" s="6">
+        <v>4</v>
+      </c>
+      <c r="J12" s="6">
+        <v>406</v>
+      </c>
+      <c r="K12" s="4">
+        <v>9</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C13" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D13" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
+      <c r="B13" s="6">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C13" s="6">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="D13" s="6">
+        <f t="shared" si="2"/>
+        <v>127</v>
+      </c>
+      <c r="E13" s="6">
+        <v>0</v>
+      </c>
+      <c r="F13" s="6">
+        <v>3</v>
+      </c>
+      <c r="G13" s="6">
+        <v>94</v>
+      </c>
+      <c r="H13" s="6">
+        <v>0</v>
+      </c>
+      <c r="I13" s="6">
+        <v>1</v>
+      </c>
+      <c r="J13" s="6">
+        <v>24</v>
+      </c>
+      <c r="K13" s="4">
+        <v>8</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C14" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D14" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
+      <c r="B14" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C14" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D14" s="6">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="E14" s="6">
+        <v>0</v>
+      </c>
+      <c r="F14" s="6">
+        <v>0</v>
+      </c>
+      <c r="G14" s="6">
+        <v>25</v>
+      </c>
+      <c r="H14" s="6">
+        <v>0</v>
+      </c>
+      <c r="I14" s="6">
+        <v>0</v>
+      </c>
+      <c r="J14" s="6">
+        <v>0</v>
+      </c>
+      <c r="K14" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C15" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D15" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
+      <c r="B15" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C15" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D15" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E15" s="6">
+        <v>0</v>
+      </c>
+      <c r="F15" s="6">
+        <v>0</v>
+      </c>
+      <c r="G15" s="6">
+        <v>0</v>
+      </c>
+      <c r="H15" s="6">
+        <v>0</v>
+      </c>
+      <c r="I15" s="6">
+        <v>0</v>
+      </c>
+      <c r="J15" s="6">
+        <v>0</v>
+      </c>
+      <c r="K15" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+    </row>
+    <row r="17" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+    </row>
+    <row r="18" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -937,7 +1128,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" sqref="A1:K15"/>
+      <selection pane="topRight" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1806,7 +1997,7 @@
       <c r="J8" s="2">
         <v>1</v>
       </c>
-      <c r="K8" s="7">
+      <c r="K8" s="6">
         <v>0</v>
       </c>
     </row>
@@ -1882,7 +2073,7 @@
       <c r="J10" s="2">
         <v>5</v>
       </c>
-      <c r="K10" s="7">
+      <c r="K10" s="6">
         <v>0</v>
       </c>
     </row>
@@ -1920,7 +2111,7 @@
       <c r="J11" s="2">
         <v>16</v>
       </c>
-      <c r="K11" s="7">
+      <c r="K11" s="6">
         <v>0</v>
       </c>
     </row>
@@ -1996,7 +2187,7 @@
       <c r="J13" s="2">
         <v>1</v>
       </c>
-      <c r="K13" s="7">
+      <c r="K13" s="6">
         <v>0</v>
       </c>
     </row>
@@ -2034,7 +2225,7 @@
       <c r="J14" s="2">
         <v>0</v>
       </c>
-      <c r="K14" s="7">
+      <c r="K14" s="6">
         <v>0</v>
       </c>
     </row>
@@ -2072,12 +2263,12 @@
       <c r="J15" s="2">
         <v>0</v>
       </c>
-      <c r="K15" s="7">
+      <c r="K15" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="K16" s="8"/>
+      <c r="K16" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2480,7 +2671,7 @@
       <c r="J10" s="2">
         <v>3</v>
       </c>
-      <c r="K10" s="7">
+      <c r="K10" s="6">
         <v>0</v>
       </c>
     </row>
@@ -2632,7 +2823,7 @@
       <c r="J14" s="2">
         <v>0</v>
       </c>
-      <c r="K14" s="7">
+      <c r="K14" s="6">
         <v>0</v>
       </c>
     </row>
@@ -2670,7 +2861,7 @@
       <c r="J15" s="2">
         <v>0</v>
       </c>
-      <c r="K15" s="7">
+      <c r="K15" s="6">
         <v>0</v>
       </c>
     </row>

</xml_diff>